<commit_message>
Entrega Prototipo + Correcoes
</commit_message>
<xml_diff>
--- a/02.Requisitos funcionais/REQUISITOS FUNCIONAIS - JAVA-LIDAY.xlsx
+++ b/02.Requisitos funcionais/REQUISITOS FUNCIONAIS - JAVA-LIDAY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/855df28f574bbfe6/Área de Trabalho/ADS/REP-GIT/Java-liday/02.Requisitos funcionais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{0A66CC69-5BD9-478D-81DE-C5CFD0CDA96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7C3DFC1-15C1-4388-864E-11C3C67C6418}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{0A66CC69-5BD9-478D-81DE-C5CFD0CDA96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50E632A5-95AC-450E-8FF8-0ED411B81274}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4ABF0B59-3EAA-4472-9014-1459B26A9A3B}"/>
   </bookViews>
@@ -329,13 +329,13 @@
     <t>Usuário pode alterar senha a partir de usuário e email</t>
   </si>
   <si>
-    <t>DATA: 23/09/2025</t>
-  </si>
-  <si>
     <t>Recuperar senha</t>
   </si>
   <si>
     <t>Sistema envia e-mail com código de confirmação para primeiro login.</t>
+  </si>
+  <si>
+    <t>DATA: 28/10/2025</t>
   </si>
 </sst>
 </file>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3837308E-2BE3-4051-9282-618B7392BE50}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,7 +822,7 @@
     </row>
     <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1"/>
     </row>
@@ -877,7 +877,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>8</v>
@@ -991,7 +991,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>52</v>
@@ -1088,12 +1088,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010046C0C4FE9B648F44981F210CC4895080" ma:contentTypeVersion="0" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="ea081297845bd8da37d411c41c8d0221">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="574c6ccb71ee63fbc30cff3237551ec3">
     <xsd:element name="properties">
@@ -1207,6 +1201,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9030A888-F94C-446A-AE50-538902A00351}">
   <ds:schemaRefs>
@@ -1216,15 +1216,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9386896A-91B6-4EC7-AC94-350129FCA8CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FC591C5-275D-472E-91DB-ABCDD82F11B9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1238,4 +1229,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9386896A-91B6-4EC7-AC94-350129FCA8CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>